<commit_message>
added allocrule tests and removed redundant tests
</commit_message>
<xml_diff>
--- a/ftest/data/fm19/Worked_example_single_level_allocrule_2.xlsx
+++ b/ftest/data/fm19/Worked_example_single_level_allocrule_2.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\data\fm19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm19\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{244F66A7-4376-4219-8568-87658636B1CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18960" windowHeight="8664"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18960" windowHeight="8664" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="13" r:id="rId1"/>
     <sheet name="Policy Calculation" sheetId="11" r:id="rId2"/>
     <sheet name="Oasis Implementation" sheetId="12" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="146">
   <si>
     <t>Limit</t>
   </si>
@@ -552,9 +553,6 @@
   </si>
   <si>
     <t>DEDUCTIBLE_PROP_OF_LIMIT</t>
-  </si>
-  <si>
-    <t>Back Allocated Insured Loss</t>
   </si>
   <si>
     <r>
@@ -663,16 +661,22 @@
   <si>
     <t xml:space="preserve">A deductible and limit is applied to the sum of the ground up losses across all coverages and locations at the policy level, and then back-allocated to coverage. </t>
   </si>
+  <si>
+    <t>Back-allocation allocrule 1 (GU)</t>
+  </si>
+  <si>
+    <t>Back-allocation allocrule 2 (Prior Level)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,6 +778,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -929,9 +939,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1049,16 +1059,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1073,15 +1074,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1090,6 +1082,21 @@
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1431,10 +1438,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1474,7 +1481,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1563,8 +1570,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" location="'Policy Calculation'!A1" display="Policy calculation"/>
-    <hyperlink ref="A17" location="'Oasis Implementation'!A1" display="Oasis Implementation"/>
+    <hyperlink ref="A15" location="'Policy Calculation'!A1" display="Policy calculation" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A17" location="'Oasis Implementation'!A1" display="Oasis Implementation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1572,14 +1579,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1611,7 +1618,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1756,7 +1763,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -1799,20 +1806,20 @@
     <row r="35" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="B35" s="49"/>
-      <c r="C35" s="65" t="s">
+      <c r="C35" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
-      <c r="I35" s="65" t="s">
+      <c r="I35" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="J35" s="65"/>
-      <c r="K35" s="65"/>
-      <c r="L35" s="65"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="59"/>
       <c r="M35" s="49"/>
       <c r="N35" s="50" t="s">
         <v>110</v>
@@ -1935,19 +1942,19 @@
       <c r="B40" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="57"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="54"/>
       <c r="M40" s="43"/>
       <c r="N40" s="43"/>
-      <c r="O40" s="59"/>
+      <c r="O40" s="56"/>
     </row>
     <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="36" t="s">
@@ -1956,18 +1963,18 @@
       <c r="B41" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="57"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
       <c r="M41" s="43"/>
-      <c r="N41" s="56">
+      <c r="N41" s="53">
         <v>50000</v>
       </c>
     </row>
@@ -1978,18 +1985,18 @@
       <c r="B42" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
       <c r="M42" s="43"/>
-      <c r="N42" s="56">
+      <c r="N42" s="53">
         <v>2500000</v>
       </c>
     </row>
@@ -2146,30 +2153,30 @@
         <v>336900</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1025" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="55"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="55"/>
       <c r="M49" s="43"/>
       <c r="N49" s="52">
         <f>N48</f>
         <v>336900</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1025" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="36" t="s">
         <v>115</v>
       </c>
@@ -2192,114 +2199,2173 @@
         <v>286900</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1025" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="36" t="s">
         <v>123</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
       <c r="M51" s="43"/>
       <c r="N51" s="52">
         <f>MIN(N42,N50)</f>
         <v>286900</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="36" t="s">
+    <row r="52" spans="1:1025" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="63" t="s">
         <v>107</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="60"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
       <c r="M52" s="43"/>
-      <c r="N52" s="55">
+      <c r="N52" s="52">
         <f>N51</f>
         <v>286900</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="C53" s="62">
-        <f>$N$52*C48/$N$48</f>
+    <row r="53" spans="1:1025" x14ac:dyDescent="0.3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="65"/>
+    </row>
+    <row r="54" spans="1:1025" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="61"/>
+      <c r="C54" s="62">
+        <f>C$48*$N$52/$N$48</f>
         <v>85158.800831107146</v>
       </c>
-      <c r="D53" s="62">
-        <f>$N$52*D48/$N$48</f>
+      <c r="D54" s="62">
+        <f t="shared" ref="D54:F55" si="2">D$48*$N$52/$N$48</f>
         <v>8515.8800831107146</v>
       </c>
-      <c r="E53" s="62">
-        <f>$N$52*E48/$N$48</f>
+      <c r="E54" s="62">
+        <f t="shared" si="2"/>
         <v>2128.9700207776787</v>
       </c>
-      <c r="F53" s="62">
-        <f>$N$52*F48/$N$48</f>
+      <c r="F54" s="62">
+        <f t="shared" si="2"/>
         <v>340.63520332442863</v>
       </c>
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="62">
-        <f>$N$52*I48/$N$48</f>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="62">
+        <f>I$48*$N$52/$N$48</f>
         <v>144769.96141288217</v>
       </c>
-      <c r="J53" s="62">
-        <f>$N$52*J48/$N$48</f>
+      <c r="J54" s="62">
+        <f t="shared" ref="J54:L55" si="3">J$48*$N$52/$N$48</f>
         <v>2554.7640249332144</v>
       </c>
-      <c r="K53" s="62">
-        <f>$N$52*K48/$N$48</f>
+      <c r="K54" s="62">
+        <f t="shared" si="3"/>
         <v>42579.400415553573</v>
       </c>
-      <c r="L53" s="62">
-        <f>$N$52*L48/$N$48</f>
+      <c r="L54" s="62">
+        <f t="shared" si="3"/>
         <v>851.58800831107158</v>
       </c>
-      <c r="M53" s="62"/>
-      <c r="N53" s="55">
-        <f>N51</f>
-        <v>286900</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="58"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AB54" s="2"/>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="2"/>
+      <c r="AF54" s="2"/>
+      <c r="AG54" s="2"/>
+      <c r="AH54" s="2"/>
+      <c r="AI54" s="2"/>
+      <c r="AJ54" s="2"/>
+      <c r="AK54" s="2"/>
+      <c r="AL54" s="2"/>
+      <c r="AM54" s="2"/>
+      <c r="AN54" s="2"/>
+      <c r="AO54" s="2"/>
+      <c r="AP54" s="2"/>
+      <c r="AQ54" s="2"/>
+      <c r="AR54" s="2"/>
+      <c r="AS54" s="2"/>
+      <c r="AT54" s="2"/>
+      <c r="AU54" s="2"/>
+      <c r="AV54" s="2"/>
+      <c r="AW54" s="2"/>
+      <c r="AX54" s="2"/>
+      <c r="AY54" s="2"/>
+      <c r="AZ54" s="2"/>
+      <c r="BA54" s="2"/>
+      <c r="BB54" s="2"/>
+      <c r="BC54" s="2"/>
+      <c r="BD54" s="2"/>
+      <c r="BE54" s="2"/>
+      <c r="BF54" s="2"/>
+      <c r="BG54" s="2"/>
+      <c r="BH54" s="2"/>
+      <c r="BI54" s="2"/>
+      <c r="BJ54" s="2"/>
+      <c r="BK54" s="2"/>
+      <c r="BL54" s="2"/>
+      <c r="BM54" s="2"/>
+      <c r="BN54" s="2"/>
+      <c r="BO54" s="2"/>
+      <c r="BP54" s="2"/>
+      <c r="BQ54" s="2"/>
+      <c r="BR54" s="2"/>
+      <c r="BS54" s="2"/>
+      <c r="BT54" s="2"/>
+      <c r="BU54" s="2"/>
+      <c r="BV54" s="2"/>
+      <c r="BW54" s="2"/>
+      <c r="BX54" s="2"/>
+      <c r="BY54" s="2"/>
+      <c r="BZ54" s="2"/>
+      <c r="CA54" s="2"/>
+      <c r="CB54" s="2"/>
+      <c r="CC54" s="2"/>
+      <c r="CD54" s="2"/>
+      <c r="CE54" s="2"/>
+      <c r="CF54" s="2"/>
+      <c r="CG54" s="2"/>
+      <c r="CH54" s="2"/>
+      <c r="CI54" s="2"/>
+      <c r="CJ54" s="2"/>
+      <c r="CK54" s="2"/>
+      <c r="CL54" s="2"/>
+      <c r="CM54" s="2"/>
+      <c r="CN54" s="2"/>
+      <c r="CO54" s="2"/>
+      <c r="CP54" s="2"/>
+      <c r="CQ54" s="2"/>
+      <c r="CR54" s="2"/>
+      <c r="CS54" s="2"/>
+      <c r="CT54" s="2"/>
+      <c r="CU54" s="2"/>
+      <c r="CV54" s="2"/>
+      <c r="CW54" s="2"/>
+      <c r="CX54" s="2"/>
+      <c r="CY54" s="2"/>
+      <c r="CZ54" s="2"/>
+      <c r="DA54" s="2"/>
+      <c r="DB54" s="2"/>
+      <c r="DC54" s="2"/>
+      <c r="DD54" s="2"/>
+      <c r="DE54" s="2"/>
+      <c r="DF54" s="2"/>
+      <c r="DG54" s="2"/>
+      <c r="DH54" s="2"/>
+      <c r="DI54" s="2"/>
+      <c r="DJ54" s="2"/>
+      <c r="DK54" s="2"/>
+      <c r="DL54" s="2"/>
+      <c r="DM54" s="2"/>
+      <c r="DN54" s="2"/>
+      <c r="DO54" s="2"/>
+      <c r="DP54" s="2"/>
+      <c r="DQ54" s="2"/>
+      <c r="DR54" s="2"/>
+      <c r="DS54" s="2"/>
+      <c r="DT54" s="2"/>
+      <c r="DU54" s="2"/>
+      <c r="DV54" s="2"/>
+      <c r="DW54" s="2"/>
+      <c r="DX54" s="2"/>
+      <c r="DY54" s="2"/>
+      <c r="DZ54" s="2"/>
+      <c r="EA54" s="2"/>
+      <c r="EB54" s="2"/>
+      <c r="EC54" s="2"/>
+      <c r="ED54" s="2"/>
+      <c r="EE54" s="2"/>
+      <c r="EF54" s="2"/>
+      <c r="EG54" s="2"/>
+      <c r="EH54" s="2"/>
+      <c r="EI54" s="2"/>
+      <c r="EJ54" s="2"/>
+      <c r="EK54" s="2"/>
+      <c r="EL54" s="2"/>
+      <c r="EM54" s="2"/>
+      <c r="EN54" s="2"/>
+      <c r="EO54" s="2"/>
+      <c r="EP54" s="2"/>
+      <c r="EQ54" s="2"/>
+      <c r="ER54" s="2"/>
+      <c r="ES54" s="2"/>
+      <c r="ET54" s="2"/>
+      <c r="EU54" s="2"/>
+      <c r="EV54" s="2"/>
+      <c r="EW54" s="2"/>
+      <c r="EX54" s="2"/>
+      <c r="EY54" s="2"/>
+      <c r="EZ54" s="2"/>
+      <c r="FA54" s="2"/>
+      <c r="FB54" s="2"/>
+      <c r="FC54" s="2"/>
+      <c r="FD54" s="2"/>
+      <c r="FE54" s="2"/>
+      <c r="FF54" s="2"/>
+      <c r="FG54" s="2"/>
+      <c r="FH54" s="2"/>
+      <c r="FI54" s="2"/>
+      <c r="FJ54" s="2"/>
+      <c r="FK54" s="2"/>
+      <c r="FL54" s="2"/>
+      <c r="FM54" s="2"/>
+      <c r="FN54" s="2"/>
+      <c r="FO54" s="2"/>
+      <c r="FP54" s="2"/>
+      <c r="FQ54" s="2"/>
+      <c r="FR54" s="2"/>
+      <c r="FS54" s="2"/>
+      <c r="FT54" s="2"/>
+      <c r="FU54" s="2"/>
+      <c r="FV54" s="2"/>
+      <c r="FW54" s="2"/>
+      <c r="FX54" s="2"/>
+      <c r="FY54" s="2"/>
+      <c r="FZ54" s="2"/>
+      <c r="GA54" s="2"/>
+      <c r="GB54" s="2"/>
+      <c r="GC54" s="2"/>
+      <c r="GD54" s="2"/>
+      <c r="GE54" s="2"/>
+      <c r="GF54" s="2"/>
+      <c r="GG54" s="2"/>
+      <c r="GH54" s="2"/>
+      <c r="GI54" s="2"/>
+      <c r="GJ54" s="2"/>
+      <c r="GK54" s="2"/>
+      <c r="GL54" s="2"/>
+      <c r="GM54" s="2"/>
+      <c r="GN54" s="2"/>
+      <c r="GO54" s="2"/>
+      <c r="GP54" s="2"/>
+      <c r="GQ54" s="2"/>
+      <c r="GR54" s="2"/>
+      <c r="GS54" s="2"/>
+      <c r="GT54" s="2"/>
+      <c r="GU54" s="2"/>
+      <c r="GV54" s="2"/>
+      <c r="GW54" s="2"/>
+      <c r="GX54" s="2"/>
+      <c r="GY54" s="2"/>
+      <c r="GZ54" s="2"/>
+      <c r="HA54" s="2"/>
+      <c r="HB54" s="2"/>
+      <c r="HC54" s="2"/>
+      <c r="HD54" s="2"/>
+      <c r="HE54" s="2"/>
+      <c r="HF54" s="2"/>
+      <c r="HG54" s="2"/>
+      <c r="HH54" s="2"/>
+      <c r="HI54" s="2"/>
+      <c r="HJ54" s="2"/>
+      <c r="HK54" s="2"/>
+      <c r="HL54" s="2"/>
+      <c r="HM54" s="2"/>
+      <c r="HN54" s="2"/>
+      <c r="HO54" s="2"/>
+      <c r="HP54" s="2"/>
+      <c r="HQ54" s="2"/>
+      <c r="HR54" s="2"/>
+      <c r="HS54" s="2"/>
+      <c r="HT54" s="2"/>
+      <c r="HU54" s="2"/>
+      <c r="HV54" s="2"/>
+      <c r="HW54" s="2"/>
+      <c r="HX54" s="2"/>
+      <c r="HY54" s="2"/>
+      <c r="HZ54" s="2"/>
+      <c r="IA54" s="2"/>
+      <c r="IB54" s="2"/>
+      <c r="IC54" s="2"/>
+      <c r="ID54" s="2"/>
+      <c r="IE54" s="2"/>
+      <c r="IF54" s="2"/>
+      <c r="IG54" s="2"/>
+      <c r="IH54" s="2"/>
+      <c r="II54" s="2"/>
+      <c r="IJ54" s="2"/>
+      <c r="IK54" s="2"/>
+      <c r="IL54" s="2"/>
+      <c r="IM54" s="2"/>
+      <c r="IN54" s="2"/>
+      <c r="IO54" s="2"/>
+      <c r="IP54" s="2"/>
+      <c r="IQ54" s="2"/>
+      <c r="IR54" s="2"/>
+      <c r="IS54" s="2"/>
+      <c r="IT54" s="2"/>
+      <c r="IU54" s="2"/>
+      <c r="IV54" s="2"/>
+      <c r="IW54" s="2"/>
+      <c r="IX54" s="2"/>
+      <c r="IY54" s="2"/>
+      <c r="IZ54" s="2"/>
+      <c r="JA54" s="2"/>
+      <c r="JB54" s="2"/>
+      <c r="JC54" s="2"/>
+      <c r="JD54" s="2"/>
+      <c r="JE54" s="2"/>
+      <c r="JF54" s="2"/>
+      <c r="JG54" s="2"/>
+      <c r="JH54" s="2"/>
+      <c r="JI54" s="2"/>
+      <c r="JJ54" s="2"/>
+      <c r="JK54" s="2"/>
+      <c r="JL54" s="2"/>
+      <c r="JM54" s="2"/>
+      <c r="JN54" s="2"/>
+      <c r="JO54" s="2"/>
+      <c r="JP54" s="2"/>
+      <c r="JQ54" s="2"/>
+      <c r="JR54" s="2"/>
+      <c r="JS54" s="2"/>
+      <c r="JT54" s="2"/>
+      <c r="JU54" s="2"/>
+      <c r="JV54" s="2"/>
+      <c r="JW54" s="2"/>
+      <c r="JX54" s="2"/>
+      <c r="JY54" s="2"/>
+      <c r="JZ54" s="2"/>
+      <c r="KA54" s="2"/>
+      <c r="KB54" s="2"/>
+      <c r="KC54" s="2"/>
+      <c r="KD54" s="2"/>
+      <c r="KE54" s="2"/>
+      <c r="KF54" s="2"/>
+      <c r="KG54" s="2"/>
+      <c r="KH54" s="2"/>
+      <c r="KI54" s="2"/>
+      <c r="KJ54" s="2"/>
+      <c r="KK54" s="2"/>
+      <c r="KL54" s="2"/>
+      <c r="KM54" s="2"/>
+      <c r="KN54" s="2"/>
+      <c r="KO54" s="2"/>
+      <c r="KP54" s="2"/>
+      <c r="KQ54" s="2"/>
+      <c r="KR54" s="2"/>
+      <c r="KS54" s="2"/>
+      <c r="KT54" s="2"/>
+      <c r="KU54" s="2"/>
+      <c r="KV54" s="2"/>
+      <c r="KW54" s="2"/>
+      <c r="KX54" s="2"/>
+      <c r="KY54" s="2"/>
+      <c r="KZ54" s="2"/>
+      <c r="LA54" s="2"/>
+      <c r="LB54" s="2"/>
+      <c r="LC54" s="2"/>
+      <c r="LD54" s="2"/>
+      <c r="LE54" s="2"/>
+      <c r="LF54" s="2"/>
+      <c r="LG54" s="2"/>
+      <c r="LH54" s="2"/>
+      <c r="LI54" s="2"/>
+      <c r="LJ54" s="2"/>
+      <c r="LK54" s="2"/>
+      <c r="LL54" s="2"/>
+      <c r="LM54" s="2"/>
+      <c r="LN54" s="2"/>
+      <c r="LO54" s="2"/>
+      <c r="LP54" s="2"/>
+      <c r="LQ54" s="2"/>
+      <c r="LR54" s="2"/>
+      <c r="LS54" s="2"/>
+      <c r="LT54" s="2"/>
+      <c r="LU54" s="2"/>
+      <c r="LV54" s="2"/>
+      <c r="LW54" s="2"/>
+      <c r="LX54" s="2"/>
+      <c r="LY54" s="2"/>
+      <c r="LZ54" s="2"/>
+      <c r="MA54" s="2"/>
+      <c r="MB54" s="2"/>
+      <c r="MC54" s="2"/>
+      <c r="MD54" s="2"/>
+      <c r="ME54" s="2"/>
+      <c r="MF54" s="2"/>
+      <c r="MG54" s="2"/>
+      <c r="MH54" s="2"/>
+      <c r="MI54" s="2"/>
+      <c r="MJ54" s="2"/>
+      <c r="MK54" s="2"/>
+      <c r="ML54" s="2"/>
+      <c r="MM54" s="2"/>
+      <c r="MN54" s="2"/>
+      <c r="MO54" s="2"/>
+      <c r="MP54" s="2"/>
+      <c r="MQ54" s="2"/>
+      <c r="MR54" s="2"/>
+      <c r="MS54" s="2"/>
+      <c r="MT54" s="2"/>
+      <c r="MU54" s="2"/>
+      <c r="MV54" s="2"/>
+      <c r="MW54" s="2"/>
+      <c r="MX54" s="2"/>
+      <c r="MY54" s="2"/>
+      <c r="MZ54" s="2"/>
+      <c r="NA54" s="2"/>
+      <c r="NB54" s="2"/>
+      <c r="NC54" s="2"/>
+      <c r="ND54" s="2"/>
+      <c r="NE54" s="2"/>
+      <c r="NF54" s="2"/>
+      <c r="NG54" s="2"/>
+      <c r="NH54" s="2"/>
+      <c r="NI54" s="2"/>
+      <c r="NJ54" s="2"/>
+      <c r="NK54" s="2"/>
+      <c r="NL54" s="2"/>
+      <c r="NM54" s="2"/>
+      <c r="NN54" s="2"/>
+      <c r="NO54" s="2"/>
+      <c r="NP54" s="2"/>
+      <c r="NQ54" s="2"/>
+      <c r="NR54" s="2"/>
+      <c r="NS54" s="2"/>
+      <c r="NT54" s="2"/>
+      <c r="NU54" s="2"/>
+      <c r="NV54" s="2"/>
+      <c r="NW54" s="2"/>
+      <c r="NX54" s="2"/>
+      <c r="NY54" s="2"/>
+      <c r="NZ54" s="2"/>
+      <c r="OA54" s="2"/>
+      <c r="OB54" s="2"/>
+      <c r="OC54" s="2"/>
+      <c r="OD54" s="2"/>
+      <c r="OE54" s="2"/>
+      <c r="OF54" s="2"/>
+      <c r="OG54" s="2"/>
+      <c r="OH54" s="2"/>
+      <c r="OI54" s="2"/>
+      <c r="OJ54" s="2"/>
+      <c r="OK54" s="2"/>
+      <c r="OL54" s="2"/>
+      <c r="OM54" s="2"/>
+      <c r="ON54" s="2"/>
+      <c r="OO54" s="2"/>
+      <c r="OP54" s="2"/>
+      <c r="OQ54" s="2"/>
+      <c r="OR54" s="2"/>
+      <c r="OS54" s="2"/>
+      <c r="OT54" s="2"/>
+      <c r="OU54" s="2"/>
+      <c r="OV54" s="2"/>
+      <c r="OW54" s="2"/>
+      <c r="OX54" s="2"/>
+      <c r="OY54" s="2"/>
+      <c r="OZ54" s="2"/>
+      <c r="PA54" s="2"/>
+      <c r="PB54" s="2"/>
+      <c r="PC54" s="2"/>
+      <c r="PD54" s="2"/>
+      <c r="PE54" s="2"/>
+      <c r="PF54" s="2"/>
+      <c r="PG54" s="2"/>
+      <c r="PH54" s="2"/>
+      <c r="PI54" s="2"/>
+      <c r="PJ54" s="2"/>
+      <c r="PK54" s="2"/>
+      <c r="PL54" s="2"/>
+      <c r="PM54" s="2"/>
+      <c r="PN54" s="2"/>
+      <c r="PO54" s="2"/>
+      <c r="PP54" s="2"/>
+      <c r="PQ54" s="2"/>
+      <c r="PR54" s="2"/>
+      <c r="PS54" s="2"/>
+      <c r="PT54" s="2"/>
+      <c r="PU54" s="2"/>
+      <c r="PV54" s="2"/>
+      <c r="PW54" s="2"/>
+      <c r="PX54" s="2"/>
+      <c r="PY54" s="2"/>
+      <c r="PZ54" s="2"/>
+      <c r="QA54" s="2"/>
+      <c r="QB54" s="2"/>
+      <c r="QC54" s="2"/>
+      <c r="QD54" s="2"/>
+      <c r="QE54" s="2"/>
+      <c r="QF54" s="2"/>
+      <c r="QG54" s="2"/>
+      <c r="QH54" s="2"/>
+      <c r="QI54" s="2"/>
+      <c r="QJ54" s="2"/>
+      <c r="QK54" s="2"/>
+      <c r="QL54" s="2"/>
+      <c r="QM54" s="2"/>
+      <c r="QN54" s="2"/>
+      <c r="QO54" s="2"/>
+      <c r="QP54" s="2"/>
+      <c r="QQ54" s="2"/>
+      <c r="QR54" s="2"/>
+      <c r="QS54" s="2"/>
+      <c r="QT54" s="2"/>
+      <c r="QU54" s="2"/>
+      <c r="QV54" s="2"/>
+      <c r="QW54" s="2"/>
+      <c r="QX54" s="2"/>
+      <c r="QY54" s="2"/>
+      <c r="QZ54" s="2"/>
+      <c r="RA54" s="2"/>
+      <c r="RB54" s="2"/>
+      <c r="RC54" s="2"/>
+      <c r="RD54" s="2"/>
+      <c r="RE54" s="2"/>
+      <c r="RF54" s="2"/>
+      <c r="RG54" s="2"/>
+      <c r="RH54" s="2"/>
+      <c r="RI54" s="2"/>
+      <c r="RJ54" s="2"/>
+      <c r="RK54" s="2"/>
+      <c r="RL54" s="2"/>
+      <c r="RM54" s="2"/>
+      <c r="RN54" s="2"/>
+      <c r="RO54" s="2"/>
+      <c r="RP54" s="2"/>
+      <c r="RQ54" s="2"/>
+      <c r="RR54" s="2"/>
+      <c r="RS54" s="2"/>
+      <c r="RT54" s="2"/>
+      <c r="RU54" s="2"/>
+      <c r="RV54" s="2"/>
+      <c r="RW54" s="2"/>
+      <c r="RX54" s="2"/>
+      <c r="RY54" s="2"/>
+      <c r="RZ54" s="2"/>
+      <c r="SA54" s="2"/>
+      <c r="SB54" s="2"/>
+      <c r="SC54" s="2"/>
+      <c r="SD54" s="2"/>
+      <c r="SE54" s="2"/>
+      <c r="SF54" s="2"/>
+      <c r="SG54" s="2"/>
+      <c r="SH54" s="2"/>
+      <c r="SI54" s="2"/>
+      <c r="SJ54" s="2"/>
+      <c r="SK54" s="2"/>
+      <c r="SL54" s="2"/>
+      <c r="SM54" s="2"/>
+      <c r="SN54" s="2"/>
+      <c r="SO54" s="2"/>
+      <c r="SP54" s="2"/>
+      <c r="SQ54" s="2"/>
+      <c r="SR54" s="2"/>
+      <c r="SS54" s="2"/>
+      <c r="ST54" s="2"/>
+      <c r="SU54" s="2"/>
+      <c r="SV54" s="2"/>
+      <c r="SW54" s="2"/>
+      <c r="SX54" s="2"/>
+      <c r="SY54" s="2"/>
+      <c r="SZ54" s="2"/>
+      <c r="TA54" s="2"/>
+      <c r="TB54" s="2"/>
+      <c r="TC54" s="2"/>
+      <c r="TD54" s="2"/>
+      <c r="TE54" s="2"/>
+      <c r="TF54" s="2"/>
+      <c r="TG54" s="2"/>
+      <c r="TH54" s="2"/>
+      <c r="TI54" s="2"/>
+      <c r="TJ54" s="2"/>
+      <c r="TK54" s="2"/>
+      <c r="TL54" s="2"/>
+      <c r="TM54" s="2"/>
+      <c r="TN54" s="2"/>
+      <c r="TO54" s="2"/>
+      <c r="TP54" s="2"/>
+      <c r="TQ54" s="2"/>
+      <c r="TR54" s="2"/>
+      <c r="TS54" s="2"/>
+      <c r="TT54" s="2"/>
+      <c r="TU54" s="2"/>
+      <c r="TV54" s="2"/>
+      <c r="TW54" s="2"/>
+      <c r="TX54" s="2"/>
+      <c r="TY54" s="2"/>
+      <c r="TZ54" s="2"/>
+      <c r="UA54" s="2"/>
+      <c r="UB54" s="2"/>
+      <c r="UC54" s="2"/>
+      <c r="UD54" s="2"/>
+      <c r="UE54" s="2"/>
+      <c r="UF54" s="2"/>
+      <c r="UG54" s="2"/>
+      <c r="UH54" s="2"/>
+      <c r="UI54" s="2"/>
+      <c r="UJ54" s="2"/>
+      <c r="UK54" s="2"/>
+      <c r="UL54" s="2"/>
+      <c r="UM54" s="2"/>
+      <c r="UN54" s="2"/>
+      <c r="UO54" s="2"/>
+      <c r="UP54" s="2"/>
+      <c r="UQ54" s="2"/>
+      <c r="UR54" s="2"/>
+      <c r="US54" s="2"/>
+      <c r="UT54" s="2"/>
+      <c r="UU54" s="2"/>
+      <c r="UV54" s="2"/>
+      <c r="UW54" s="2"/>
+      <c r="UX54" s="2"/>
+      <c r="UY54" s="2"/>
+      <c r="UZ54" s="2"/>
+      <c r="VA54" s="2"/>
+      <c r="VB54" s="2"/>
+      <c r="VC54" s="2"/>
+      <c r="VD54" s="2"/>
+      <c r="VE54" s="2"/>
+      <c r="VF54" s="2"/>
+      <c r="VG54" s="2"/>
+      <c r="VH54" s="2"/>
+      <c r="VI54" s="2"/>
+      <c r="VJ54" s="2"/>
+      <c r="VK54" s="2"/>
+      <c r="VL54" s="2"/>
+      <c r="VM54" s="2"/>
+      <c r="VN54" s="2"/>
+      <c r="VO54" s="2"/>
+      <c r="VP54" s="2"/>
+      <c r="VQ54" s="2"/>
+      <c r="VR54" s="2"/>
+      <c r="VS54" s="2"/>
+      <c r="VT54" s="2"/>
+      <c r="VU54" s="2"/>
+      <c r="VV54" s="2"/>
+      <c r="VW54" s="2"/>
+      <c r="VX54" s="2"/>
+      <c r="VY54" s="2"/>
+      <c r="VZ54" s="2"/>
+      <c r="WA54" s="2"/>
+      <c r="WB54" s="2"/>
+      <c r="WC54" s="2"/>
+      <c r="WD54" s="2"/>
+      <c r="WE54" s="2"/>
+      <c r="WF54" s="2"/>
+      <c r="WG54" s="2"/>
+      <c r="WH54" s="2"/>
+      <c r="WI54" s="2"/>
+      <c r="WJ54" s="2"/>
+      <c r="WK54" s="2"/>
+      <c r="WL54" s="2"/>
+      <c r="WM54" s="2"/>
+      <c r="WN54" s="2"/>
+      <c r="WO54" s="2"/>
+      <c r="WP54" s="2"/>
+      <c r="WQ54" s="2"/>
+      <c r="WR54" s="2"/>
+      <c r="WS54" s="2"/>
+      <c r="WT54" s="2"/>
+      <c r="WU54" s="2"/>
+      <c r="WV54" s="2"/>
+      <c r="WW54" s="2"/>
+      <c r="WX54" s="2"/>
+      <c r="WY54" s="2"/>
+      <c r="WZ54" s="2"/>
+      <c r="XA54" s="2"/>
+      <c r="XB54" s="2"/>
+      <c r="XC54" s="2"/>
+      <c r="XD54" s="2"/>
+      <c r="XE54" s="2"/>
+      <c r="XF54" s="2"/>
+      <c r="XG54" s="2"/>
+      <c r="XH54" s="2"/>
+      <c r="XI54" s="2"/>
+      <c r="XJ54" s="2"/>
+      <c r="XK54" s="2"/>
+      <c r="XL54" s="2"/>
+      <c r="XM54" s="2"/>
+      <c r="XN54" s="2"/>
+      <c r="XO54" s="2"/>
+      <c r="XP54" s="2"/>
+      <c r="XQ54" s="2"/>
+      <c r="XR54" s="2"/>
+      <c r="XS54" s="2"/>
+      <c r="XT54" s="2"/>
+      <c r="XU54" s="2"/>
+      <c r="XV54" s="2"/>
+      <c r="XW54" s="2"/>
+      <c r="XX54" s="2"/>
+      <c r="XY54" s="2"/>
+      <c r="XZ54" s="2"/>
+      <c r="YA54" s="2"/>
+      <c r="YB54" s="2"/>
+      <c r="YC54" s="2"/>
+      <c r="YD54" s="2"/>
+      <c r="YE54" s="2"/>
+      <c r="YF54" s="2"/>
+      <c r="YG54" s="2"/>
+      <c r="YH54" s="2"/>
+      <c r="YI54" s="2"/>
+      <c r="YJ54" s="2"/>
+      <c r="YK54" s="2"/>
+      <c r="YL54" s="2"/>
+      <c r="YM54" s="2"/>
+      <c r="YN54" s="2"/>
+      <c r="YO54" s="2"/>
+      <c r="YP54" s="2"/>
+      <c r="YQ54" s="2"/>
+      <c r="YR54" s="2"/>
+      <c r="YS54" s="2"/>
+      <c r="YT54" s="2"/>
+      <c r="YU54" s="2"/>
+      <c r="YV54" s="2"/>
+      <c r="YW54" s="2"/>
+      <c r="YX54" s="2"/>
+      <c r="YY54" s="2"/>
+      <c r="YZ54" s="2"/>
+      <c r="ZA54" s="2"/>
+      <c r="ZB54" s="2"/>
+      <c r="ZC54" s="2"/>
+      <c r="ZD54" s="2"/>
+      <c r="ZE54" s="2"/>
+      <c r="ZF54" s="2"/>
+      <c r="ZG54" s="2"/>
+      <c r="ZH54" s="2"/>
+      <c r="ZI54" s="2"/>
+      <c r="ZJ54" s="2"/>
+      <c r="ZK54" s="2"/>
+      <c r="ZL54" s="2"/>
+      <c r="ZM54" s="2"/>
+      <c r="ZN54" s="2"/>
+      <c r="ZO54" s="2"/>
+      <c r="ZP54" s="2"/>
+      <c r="ZQ54" s="2"/>
+      <c r="ZR54" s="2"/>
+      <c r="ZS54" s="2"/>
+      <c r="ZT54" s="2"/>
+      <c r="ZU54" s="2"/>
+      <c r="ZV54" s="2"/>
+      <c r="ZW54" s="2"/>
+      <c r="ZX54" s="2"/>
+      <c r="ZY54" s="2"/>
+      <c r="ZZ54" s="2"/>
+      <c r="AAA54" s="2"/>
+      <c r="AAB54" s="2"/>
+      <c r="AAC54" s="2"/>
+      <c r="AAD54" s="2"/>
+      <c r="AAE54" s="2"/>
+      <c r="AAF54" s="2"/>
+      <c r="AAG54" s="2"/>
+      <c r="AAH54" s="2"/>
+      <c r="AAI54" s="2"/>
+      <c r="AAJ54" s="2"/>
+      <c r="AAK54" s="2"/>
+      <c r="AAL54" s="2"/>
+      <c r="AAM54" s="2"/>
+      <c r="AAN54" s="2"/>
+      <c r="AAO54" s="2"/>
+      <c r="AAP54" s="2"/>
+      <c r="AAQ54" s="2"/>
+      <c r="AAR54" s="2"/>
+      <c r="AAS54" s="2"/>
+      <c r="AAT54" s="2"/>
+      <c r="AAU54" s="2"/>
+      <c r="AAV54" s="2"/>
+      <c r="AAW54" s="2"/>
+      <c r="AAX54" s="2"/>
+      <c r="AAY54" s="2"/>
+      <c r="AAZ54" s="2"/>
+      <c r="ABA54" s="2"/>
+      <c r="ABB54" s="2"/>
+      <c r="ABC54" s="2"/>
+      <c r="ABD54" s="2"/>
+      <c r="ABE54" s="2"/>
+      <c r="ABF54" s="2"/>
+      <c r="ABG54" s="2"/>
+      <c r="ABH54" s="2"/>
+      <c r="ABI54" s="2"/>
+      <c r="ABJ54" s="2"/>
+      <c r="ABK54" s="2"/>
+      <c r="ABL54" s="2"/>
+      <c r="ABM54" s="2"/>
+      <c r="ABN54" s="2"/>
+      <c r="ABO54" s="2"/>
+      <c r="ABP54" s="2"/>
+      <c r="ABQ54" s="2"/>
+      <c r="ABR54" s="2"/>
+      <c r="ABS54" s="2"/>
+      <c r="ABT54" s="2"/>
+      <c r="ABU54" s="2"/>
+      <c r="ABV54" s="2"/>
+      <c r="ABW54" s="2"/>
+      <c r="ABX54" s="2"/>
+      <c r="ABY54" s="2"/>
+      <c r="ABZ54" s="2"/>
+      <c r="ACA54" s="2"/>
+      <c r="ACB54" s="2"/>
+      <c r="ACC54" s="2"/>
+      <c r="ACD54" s="2"/>
+      <c r="ACE54" s="2"/>
+      <c r="ACF54" s="2"/>
+      <c r="ACG54" s="2"/>
+      <c r="ACH54" s="2"/>
+      <c r="ACI54" s="2"/>
+      <c r="ACJ54" s="2"/>
+      <c r="ACK54" s="2"/>
+      <c r="ACL54" s="2"/>
+      <c r="ACM54" s="2"/>
+      <c r="ACN54" s="2"/>
+      <c r="ACO54" s="2"/>
+      <c r="ACP54" s="2"/>
+      <c r="ACQ54" s="2"/>
+      <c r="ACR54" s="2"/>
+      <c r="ACS54" s="2"/>
+      <c r="ACT54" s="2"/>
+      <c r="ACU54" s="2"/>
+      <c r="ACV54" s="2"/>
+      <c r="ACW54" s="2"/>
+      <c r="ACX54" s="2"/>
+      <c r="ACY54" s="2"/>
+      <c r="ACZ54" s="2"/>
+      <c r="ADA54" s="2"/>
+      <c r="ADB54" s="2"/>
+      <c r="ADC54" s="2"/>
+      <c r="ADD54" s="2"/>
+      <c r="ADE54" s="2"/>
+      <c r="ADF54" s="2"/>
+      <c r="ADG54" s="2"/>
+      <c r="ADH54" s="2"/>
+      <c r="ADI54" s="2"/>
+      <c r="ADJ54" s="2"/>
+      <c r="ADK54" s="2"/>
+      <c r="ADL54" s="2"/>
+      <c r="ADM54" s="2"/>
+      <c r="ADN54" s="2"/>
+      <c r="ADO54" s="2"/>
+      <c r="ADP54" s="2"/>
+      <c r="ADQ54" s="2"/>
+      <c r="ADR54" s="2"/>
+      <c r="ADS54" s="2"/>
+      <c r="ADT54" s="2"/>
+      <c r="ADU54" s="2"/>
+      <c r="ADV54" s="2"/>
+      <c r="ADW54" s="2"/>
+      <c r="ADX54" s="2"/>
+      <c r="ADY54" s="2"/>
+      <c r="ADZ54" s="2"/>
+      <c r="AEA54" s="2"/>
+      <c r="AEB54" s="2"/>
+      <c r="AEC54" s="2"/>
+      <c r="AED54" s="2"/>
+      <c r="AEE54" s="2"/>
+      <c r="AEF54" s="2"/>
+      <c r="AEG54" s="2"/>
+      <c r="AEH54" s="2"/>
+      <c r="AEI54" s="2"/>
+      <c r="AEJ54" s="2"/>
+      <c r="AEK54" s="2"/>
+      <c r="AEL54" s="2"/>
+      <c r="AEM54" s="2"/>
+      <c r="AEN54" s="2"/>
+      <c r="AEO54" s="2"/>
+      <c r="AEP54" s="2"/>
+      <c r="AEQ54" s="2"/>
+      <c r="AER54" s="2"/>
+      <c r="AES54" s="2"/>
+      <c r="AET54" s="2"/>
+      <c r="AEU54" s="2"/>
+      <c r="AEV54" s="2"/>
+      <c r="AEW54" s="2"/>
+      <c r="AEX54" s="2"/>
+      <c r="AEY54" s="2"/>
+      <c r="AEZ54" s="2"/>
+      <c r="AFA54" s="2"/>
+      <c r="AFB54" s="2"/>
+      <c r="AFC54" s="2"/>
+      <c r="AFD54" s="2"/>
+      <c r="AFE54" s="2"/>
+      <c r="AFF54" s="2"/>
+      <c r="AFG54" s="2"/>
+      <c r="AFH54" s="2"/>
+      <c r="AFI54" s="2"/>
+      <c r="AFJ54" s="2"/>
+      <c r="AFK54" s="2"/>
+      <c r="AFL54" s="2"/>
+      <c r="AFM54" s="2"/>
+      <c r="AFN54" s="2"/>
+      <c r="AFO54" s="2"/>
+      <c r="AFP54" s="2"/>
+      <c r="AFQ54" s="2"/>
+      <c r="AFR54" s="2"/>
+      <c r="AFS54" s="2"/>
+      <c r="AFT54" s="2"/>
+      <c r="AFU54" s="2"/>
+      <c r="AFV54" s="2"/>
+      <c r="AFW54" s="2"/>
+      <c r="AFX54" s="2"/>
+      <c r="AFY54" s="2"/>
+      <c r="AFZ54" s="2"/>
+      <c r="AGA54" s="2"/>
+      <c r="AGB54" s="2"/>
+      <c r="AGC54" s="2"/>
+      <c r="AGD54" s="2"/>
+      <c r="AGE54" s="2"/>
+      <c r="AGF54" s="2"/>
+      <c r="AGG54" s="2"/>
+      <c r="AGH54" s="2"/>
+      <c r="AGI54" s="2"/>
+      <c r="AGJ54" s="2"/>
+      <c r="AGK54" s="2"/>
+      <c r="AGL54" s="2"/>
+      <c r="AGM54" s="2"/>
+      <c r="AGN54" s="2"/>
+      <c r="AGO54" s="2"/>
+      <c r="AGP54" s="2"/>
+      <c r="AGQ54" s="2"/>
+      <c r="AGR54" s="2"/>
+      <c r="AGS54" s="2"/>
+      <c r="AGT54" s="2"/>
+      <c r="AGU54" s="2"/>
+      <c r="AGV54" s="2"/>
+      <c r="AGW54" s="2"/>
+      <c r="AGX54" s="2"/>
+      <c r="AGY54" s="2"/>
+      <c r="AGZ54" s="2"/>
+      <c r="AHA54" s="2"/>
+      <c r="AHB54" s="2"/>
+      <c r="AHC54" s="2"/>
+      <c r="AHD54" s="2"/>
+      <c r="AHE54" s="2"/>
+      <c r="AHF54" s="2"/>
+      <c r="AHG54" s="2"/>
+      <c r="AHH54" s="2"/>
+      <c r="AHI54" s="2"/>
+      <c r="AHJ54" s="2"/>
+      <c r="AHK54" s="2"/>
+      <c r="AHL54" s="2"/>
+      <c r="AHM54" s="2"/>
+      <c r="AHN54" s="2"/>
+      <c r="AHO54" s="2"/>
+      <c r="AHP54" s="2"/>
+      <c r="AHQ54" s="2"/>
+      <c r="AHR54" s="2"/>
+      <c r="AHS54" s="2"/>
+      <c r="AHT54" s="2"/>
+      <c r="AHU54" s="2"/>
+      <c r="AHV54" s="2"/>
+      <c r="AHW54" s="2"/>
+      <c r="AHX54" s="2"/>
+      <c r="AHY54" s="2"/>
+      <c r="AHZ54" s="2"/>
+      <c r="AIA54" s="2"/>
+      <c r="AIB54" s="2"/>
+      <c r="AIC54" s="2"/>
+      <c r="AID54" s="2"/>
+      <c r="AIE54" s="2"/>
+      <c r="AIF54" s="2"/>
+      <c r="AIG54" s="2"/>
+      <c r="AIH54" s="2"/>
+      <c r="AII54" s="2"/>
+      <c r="AIJ54" s="2"/>
+      <c r="AIK54" s="2"/>
+      <c r="AIL54" s="2"/>
+      <c r="AIM54" s="2"/>
+      <c r="AIN54" s="2"/>
+      <c r="AIO54" s="2"/>
+      <c r="AIP54" s="2"/>
+      <c r="AIQ54" s="2"/>
+      <c r="AIR54" s="2"/>
+      <c r="AIS54" s="2"/>
+      <c r="AIT54" s="2"/>
+      <c r="AIU54" s="2"/>
+      <c r="AIV54" s="2"/>
+      <c r="AIW54" s="2"/>
+      <c r="AIX54" s="2"/>
+      <c r="AIY54" s="2"/>
+      <c r="AIZ54" s="2"/>
+      <c r="AJA54" s="2"/>
+      <c r="AJB54" s="2"/>
+      <c r="AJC54" s="2"/>
+      <c r="AJD54" s="2"/>
+      <c r="AJE54" s="2"/>
+      <c r="AJF54" s="2"/>
+      <c r="AJG54" s="2"/>
+      <c r="AJH54" s="2"/>
+      <c r="AJI54" s="2"/>
+      <c r="AJJ54" s="2"/>
+      <c r="AJK54" s="2"/>
+      <c r="AJL54" s="2"/>
+      <c r="AJM54" s="2"/>
+      <c r="AJN54" s="2"/>
+      <c r="AJO54" s="2"/>
+      <c r="AJP54" s="2"/>
+      <c r="AJQ54" s="2"/>
+      <c r="AJR54" s="2"/>
+      <c r="AJS54" s="2"/>
+      <c r="AJT54" s="2"/>
+      <c r="AJU54" s="2"/>
+      <c r="AJV54" s="2"/>
+      <c r="AJW54" s="2"/>
+      <c r="AJX54" s="2"/>
+      <c r="AJY54" s="2"/>
+      <c r="AJZ54" s="2"/>
+      <c r="AKA54" s="2"/>
+      <c r="AKB54" s="2"/>
+      <c r="AKC54" s="2"/>
+      <c r="AKD54" s="2"/>
+      <c r="AKE54" s="2"/>
+      <c r="AKF54" s="2"/>
+      <c r="AKG54" s="2"/>
+      <c r="AKH54" s="2"/>
+      <c r="AKI54" s="2"/>
+      <c r="AKJ54" s="2"/>
+      <c r="AKK54" s="2"/>
+      <c r="AKL54" s="2"/>
+      <c r="AKM54" s="2"/>
+      <c r="AKN54" s="2"/>
+      <c r="AKO54" s="2"/>
+      <c r="AKP54" s="2"/>
+      <c r="AKQ54" s="2"/>
+      <c r="AKR54" s="2"/>
+      <c r="AKS54" s="2"/>
+      <c r="AKT54" s="2"/>
+      <c r="AKU54" s="2"/>
+      <c r="AKV54" s="2"/>
+      <c r="AKW54" s="2"/>
+      <c r="AKX54" s="2"/>
+      <c r="AKY54" s="2"/>
+      <c r="AKZ54" s="2"/>
+      <c r="ALA54" s="2"/>
+      <c r="ALB54" s="2"/>
+      <c r="ALC54" s="2"/>
+      <c r="ALD54" s="2"/>
+      <c r="ALE54" s="2"/>
+      <c r="ALF54" s="2"/>
+      <c r="ALG54" s="2"/>
+      <c r="ALH54" s="2"/>
+      <c r="ALI54" s="2"/>
+      <c r="ALJ54" s="2"/>
+      <c r="ALK54" s="2"/>
+      <c r="ALL54" s="2"/>
+      <c r="ALM54" s="2"/>
+      <c r="ALN54" s="2"/>
+      <c r="ALO54" s="2"/>
+      <c r="ALP54" s="2"/>
+      <c r="ALQ54" s="2"/>
+      <c r="ALR54" s="2"/>
+      <c r="ALS54" s="2"/>
+      <c r="ALT54" s="2"/>
+      <c r="ALU54" s="2"/>
+      <c r="ALV54" s="2"/>
+      <c r="ALW54" s="2"/>
+      <c r="ALX54" s="2"/>
+      <c r="ALY54" s="2"/>
+      <c r="ALZ54" s="2"/>
+      <c r="AMA54" s="2"/>
+      <c r="AMB54" s="2"/>
+      <c r="AMC54" s="2"/>
+      <c r="AMD54" s="2"/>
+      <c r="AME54" s="2"/>
+      <c r="AMF54" s="2"/>
+      <c r="AMG54" s="2"/>
+      <c r="AMH54" s="2"/>
+      <c r="AMI54" s="2"/>
+      <c r="AMJ54" s="2"/>
+      <c r="AMK54" s="2"/>
+    </row>
+    <row r="55" spans="1:1025" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="61"/>
+      <c r="C55" s="62">
+        <f t="shared" ref="C55" si="4">C$48*$N$52/$N$48</f>
+        <v>85158.800831107146</v>
+      </c>
+      <c r="D55" s="62">
+        <f t="shared" si="2"/>
+        <v>8515.8800831107146</v>
+      </c>
+      <c r="E55" s="62">
+        <f t="shared" si="2"/>
+        <v>2128.9700207776787</v>
+      </c>
+      <c r="F55" s="62">
+        <f t="shared" si="2"/>
+        <v>340.63520332442863</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="62">
+        <f t="shared" ref="I55" si="5">I$48*$N$52/$N$48</f>
+        <v>144769.96141288217</v>
+      </c>
+      <c r="J55" s="62">
+        <f t="shared" si="3"/>
+        <v>2554.7640249332144</v>
+      </c>
+      <c r="K55" s="62">
+        <f t="shared" si="3"/>
+        <v>42579.400415553573</v>
+      </c>
+      <c r="L55" s="62">
+        <f t="shared" si="3"/>
+        <v>851.58800831107158</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+      <c r="AB55" s="2"/>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+      <c r="AG55" s="2"/>
+      <c r="AH55" s="2"/>
+      <c r="AI55" s="2"/>
+      <c r="AJ55" s="2"/>
+      <c r="AK55" s="2"/>
+      <c r="AL55" s="2"/>
+      <c r="AM55" s="2"/>
+      <c r="AN55" s="2"/>
+      <c r="AO55" s="2"/>
+      <c r="AP55" s="2"/>
+      <c r="AQ55" s="2"/>
+      <c r="AR55" s="2"/>
+      <c r="AS55" s="2"/>
+      <c r="AT55" s="2"/>
+      <c r="AU55" s="2"/>
+      <c r="AV55" s="2"/>
+      <c r="AW55" s="2"/>
+      <c r="AX55" s="2"/>
+      <c r="AY55" s="2"/>
+      <c r="AZ55" s="2"/>
+      <c r="BA55" s="2"/>
+      <c r="BB55" s="2"/>
+      <c r="BC55" s="2"/>
+      <c r="BD55" s="2"/>
+      <c r="BE55" s="2"/>
+      <c r="BF55" s="2"/>
+      <c r="BG55" s="2"/>
+      <c r="BH55" s="2"/>
+      <c r="BI55" s="2"/>
+      <c r="BJ55" s="2"/>
+      <c r="BK55" s="2"/>
+      <c r="BL55" s="2"/>
+      <c r="BM55" s="2"/>
+      <c r="BN55" s="2"/>
+      <c r="BO55" s="2"/>
+      <c r="BP55" s="2"/>
+      <c r="BQ55" s="2"/>
+      <c r="BR55" s="2"/>
+      <c r="BS55" s="2"/>
+      <c r="BT55" s="2"/>
+      <c r="BU55" s="2"/>
+      <c r="BV55" s="2"/>
+      <c r="BW55" s="2"/>
+      <c r="BX55" s="2"/>
+      <c r="BY55" s="2"/>
+      <c r="BZ55" s="2"/>
+      <c r="CA55" s="2"/>
+      <c r="CB55" s="2"/>
+      <c r="CC55" s="2"/>
+      <c r="CD55" s="2"/>
+      <c r="CE55" s="2"/>
+      <c r="CF55" s="2"/>
+      <c r="CG55" s="2"/>
+      <c r="CH55" s="2"/>
+      <c r="CI55" s="2"/>
+      <c r="CJ55" s="2"/>
+      <c r="CK55" s="2"/>
+      <c r="CL55" s="2"/>
+      <c r="CM55" s="2"/>
+      <c r="CN55" s="2"/>
+      <c r="CO55" s="2"/>
+      <c r="CP55" s="2"/>
+      <c r="CQ55" s="2"/>
+      <c r="CR55" s="2"/>
+      <c r="CS55" s="2"/>
+      <c r="CT55" s="2"/>
+      <c r="CU55" s="2"/>
+      <c r="CV55" s="2"/>
+      <c r="CW55" s="2"/>
+      <c r="CX55" s="2"/>
+      <c r="CY55" s="2"/>
+      <c r="CZ55" s="2"/>
+      <c r="DA55" s="2"/>
+      <c r="DB55" s="2"/>
+      <c r="DC55" s="2"/>
+      <c r="DD55" s="2"/>
+      <c r="DE55" s="2"/>
+      <c r="DF55" s="2"/>
+      <c r="DG55" s="2"/>
+      <c r="DH55" s="2"/>
+      <c r="DI55" s="2"/>
+      <c r="DJ55" s="2"/>
+      <c r="DK55" s="2"/>
+      <c r="DL55" s="2"/>
+      <c r="DM55" s="2"/>
+      <c r="DN55" s="2"/>
+      <c r="DO55" s="2"/>
+      <c r="DP55" s="2"/>
+      <c r="DQ55" s="2"/>
+      <c r="DR55" s="2"/>
+      <c r="DS55" s="2"/>
+      <c r="DT55" s="2"/>
+      <c r="DU55" s="2"/>
+      <c r="DV55" s="2"/>
+      <c r="DW55" s="2"/>
+      <c r="DX55" s="2"/>
+      <c r="DY55" s="2"/>
+      <c r="DZ55" s="2"/>
+      <c r="EA55" s="2"/>
+      <c r="EB55" s="2"/>
+      <c r="EC55" s="2"/>
+      <c r="ED55" s="2"/>
+      <c r="EE55" s="2"/>
+      <c r="EF55" s="2"/>
+      <c r="EG55" s="2"/>
+      <c r="EH55" s="2"/>
+      <c r="EI55" s="2"/>
+      <c r="EJ55" s="2"/>
+      <c r="EK55" s="2"/>
+      <c r="EL55" s="2"/>
+      <c r="EM55" s="2"/>
+      <c r="EN55" s="2"/>
+      <c r="EO55" s="2"/>
+      <c r="EP55" s="2"/>
+      <c r="EQ55" s="2"/>
+      <c r="ER55" s="2"/>
+      <c r="ES55" s="2"/>
+      <c r="ET55" s="2"/>
+      <c r="EU55" s="2"/>
+      <c r="EV55" s="2"/>
+      <c r="EW55" s="2"/>
+      <c r="EX55" s="2"/>
+      <c r="EY55" s="2"/>
+      <c r="EZ55" s="2"/>
+      <c r="FA55" s="2"/>
+      <c r="FB55" s="2"/>
+      <c r="FC55" s="2"/>
+      <c r="FD55" s="2"/>
+      <c r="FE55" s="2"/>
+      <c r="FF55" s="2"/>
+      <c r="FG55" s="2"/>
+      <c r="FH55" s="2"/>
+      <c r="FI55" s="2"/>
+      <c r="FJ55" s="2"/>
+      <c r="FK55" s="2"/>
+      <c r="FL55" s="2"/>
+      <c r="FM55" s="2"/>
+      <c r="FN55" s="2"/>
+      <c r="FO55" s="2"/>
+      <c r="FP55" s="2"/>
+      <c r="FQ55" s="2"/>
+      <c r="FR55" s="2"/>
+      <c r="FS55" s="2"/>
+      <c r="FT55" s="2"/>
+      <c r="FU55" s="2"/>
+      <c r="FV55" s="2"/>
+      <c r="FW55" s="2"/>
+      <c r="FX55" s="2"/>
+      <c r="FY55" s="2"/>
+      <c r="FZ55" s="2"/>
+      <c r="GA55" s="2"/>
+      <c r="GB55" s="2"/>
+      <c r="GC55" s="2"/>
+      <c r="GD55" s="2"/>
+      <c r="GE55" s="2"/>
+      <c r="GF55" s="2"/>
+      <c r="GG55" s="2"/>
+      <c r="GH55" s="2"/>
+      <c r="GI55" s="2"/>
+      <c r="GJ55" s="2"/>
+      <c r="GK55" s="2"/>
+      <c r="GL55" s="2"/>
+      <c r="GM55" s="2"/>
+      <c r="GN55" s="2"/>
+      <c r="GO55" s="2"/>
+      <c r="GP55" s="2"/>
+      <c r="GQ55" s="2"/>
+      <c r="GR55" s="2"/>
+      <c r="GS55" s="2"/>
+      <c r="GT55" s="2"/>
+      <c r="GU55" s="2"/>
+      <c r="GV55" s="2"/>
+      <c r="GW55" s="2"/>
+      <c r="GX55" s="2"/>
+      <c r="GY55" s="2"/>
+      <c r="GZ55" s="2"/>
+      <c r="HA55" s="2"/>
+      <c r="HB55" s="2"/>
+      <c r="HC55" s="2"/>
+      <c r="HD55" s="2"/>
+      <c r="HE55" s="2"/>
+      <c r="HF55" s="2"/>
+      <c r="HG55" s="2"/>
+      <c r="HH55" s="2"/>
+      <c r="HI55" s="2"/>
+      <c r="HJ55" s="2"/>
+      <c r="HK55" s="2"/>
+      <c r="HL55" s="2"/>
+      <c r="HM55" s="2"/>
+      <c r="HN55" s="2"/>
+      <c r="HO55" s="2"/>
+      <c r="HP55" s="2"/>
+      <c r="HQ55" s="2"/>
+      <c r="HR55" s="2"/>
+      <c r="HS55" s="2"/>
+      <c r="HT55" s="2"/>
+      <c r="HU55" s="2"/>
+      <c r="HV55" s="2"/>
+      <c r="HW55" s="2"/>
+      <c r="HX55" s="2"/>
+      <c r="HY55" s="2"/>
+      <c r="HZ55" s="2"/>
+      <c r="IA55" s="2"/>
+      <c r="IB55" s="2"/>
+      <c r="IC55" s="2"/>
+      <c r="ID55" s="2"/>
+      <c r="IE55" s="2"/>
+      <c r="IF55" s="2"/>
+      <c r="IG55" s="2"/>
+      <c r="IH55" s="2"/>
+      <c r="II55" s="2"/>
+      <c r="IJ55" s="2"/>
+      <c r="IK55" s="2"/>
+      <c r="IL55" s="2"/>
+      <c r="IM55" s="2"/>
+      <c r="IN55" s="2"/>
+      <c r="IO55" s="2"/>
+      <c r="IP55" s="2"/>
+      <c r="IQ55" s="2"/>
+      <c r="IR55" s="2"/>
+      <c r="IS55" s="2"/>
+      <c r="IT55" s="2"/>
+      <c r="IU55" s="2"/>
+      <c r="IV55" s="2"/>
+      <c r="IW55" s="2"/>
+      <c r="IX55" s="2"/>
+      <c r="IY55" s="2"/>
+      <c r="IZ55" s="2"/>
+      <c r="JA55" s="2"/>
+      <c r="JB55" s="2"/>
+      <c r="JC55" s="2"/>
+      <c r="JD55" s="2"/>
+      <c r="JE55" s="2"/>
+      <c r="JF55" s="2"/>
+      <c r="JG55" s="2"/>
+      <c r="JH55" s="2"/>
+      <c r="JI55" s="2"/>
+      <c r="JJ55" s="2"/>
+      <c r="JK55" s="2"/>
+      <c r="JL55" s="2"/>
+      <c r="JM55" s="2"/>
+      <c r="JN55" s="2"/>
+      <c r="JO55" s="2"/>
+      <c r="JP55" s="2"/>
+      <c r="JQ55" s="2"/>
+      <c r="JR55" s="2"/>
+      <c r="JS55" s="2"/>
+      <c r="JT55" s="2"/>
+      <c r="JU55" s="2"/>
+      <c r="JV55" s="2"/>
+      <c r="JW55" s="2"/>
+      <c r="JX55" s="2"/>
+      <c r="JY55" s="2"/>
+      <c r="JZ55" s="2"/>
+      <c r="KA55" s="2"/>
+      <c r="KB55" s="2"/>
+      <c r="KC55" s="2"/>
+      <c r="KD55" s="2"/>
+      <c r="KE55" s="2"/>
+      <c r="KF55" s="2"/>
+      <c r="KG55" s="2"/>
+      <c r="KH55" s="2"/>
+      <c r="KI55" s="2"/>
+      <c r="KJ55" s="2"/>
+      <c r="KK55" s="2"/>
+      <c r="KL55" s="2"/>
+      <c r="KM55" s="2"/>
+      <c r="KN55" s="2"/>
+      <c r="KO55" s="2"/>
+      <c r="KP55" s="2"/>
+      <c r="KQ55" s="2"/>
+      <c r="KR55" s="2"/>
+      <c r="KS55" s="2"/>
+      <c r="KT55" s="2"/>
+      <c r="KU55" s="2"/>
+      <c r="KV55" s="2"/>
+      <c r="KW55" s="2"/>
+      <c r="KX55" s="2"/>
+      <c r="KY55" s="2"/>
+      <c r="KZ55" s="2"/>
+      <c r="LA55" s="2"/>
+      <c r="LB55" s="2"/>
+      <c r="LC55" s="2"/>
+      <c r="LD55" s="2"/>
+      <c r="LE55" s="2"/>
+      <c r="LF55" s="2"/>
+      <c r="LG55" s="2"/>
+      <c r="LH55" s="2"/>
+      <c r="LI55" s="2"/>
+      <c r="LJ55" s="2"/>
+      <c r="LK55" s="2"/>
+      <c r="LL55" s="2"/>
+      <c r="LM55" s="2"/>
+      <c r="LN55" s="2"/>
+      <c r="LO55" s="2"/>
+      <c r="LP55" s="2"/>
+      <c r="LQ55" s="2"/>
+      <c r="LR55" s="2"/>
+      <c r="LS55" s="2"/>
+      <c r="LT55" s="2"/>
+      <c r="LU55" s="2"/>
+      <c r="LV55" s="2"/>
+      <c r="LW55" s="2"/>
+      <c r="LX55" s="2"/>
+      <c r="LY55" s="2"/>
+      <c r="LZ55" s="2"/>
+      <c r="MA55" s="2"/>
+      <c r="MB55" s="2"/>
+      <c r="MC55" s="2"/>
+      <c r="MD55" s="2"/>
+      <c r="ME55" s="2"/>
+      <c r="MF55" s="2"/>
+      <c r="MG55" s="2"/>
+      <c r="MH55" s="2"/>
+      <c r="MI55" s="2"/>
+      <c r="MJ55" s="2"/>
+      <c r="MK55" s="2"/>
+      <c r="ML55" s="2"/>
+      <c r="MM55" s="2"/>
+      <c r="MN55" s="2"/>
+      <c r="MO55" s="2"/>
+      <c r="MP55" s="2"/>
+      <c r="MQ55" s="2"/>
+      <c r="MR55" s="2"/>
+      <c r="MS55" s="2"/>
+      <c r="MT55" s="2"/>
+      <c r="MU55" s="2"/>
+      <c r="MV55" s="2"/>
+      <c r="MW55" s="2"/>
+      <c r="MX55" s="2"/>
+      <c r="MY55" s="2"/>
+      <c r="MZ55" s="2"/>
+      <c r="NA55" s="2"/>
+      <c r="NB55" s="2"/>
+      <c r="NC55" s="2"/>
+      <c r="ND55" s="2"/>
+      <c r="NE55" s="2"/>
+      <c r="NF55" s="2"/>
+      <c r="NG55" s="2"/>
+      <c r="NH55" s="2"/>
+      <c r="NI55" s="2"/>
+      <c r="NJ55" s="2"/>
+      <c r="NK55" s="2"/>
+      <c r="NL55" s="2"/>
+      <c r="NM55" s="2"/>
+      <c r="NN55" s="2"/>
+      <c r="NO55" s="2"/>
+      <c r="NP55" s="2"/>
+      <c r="NQ55" s="2"/>
+      <c r="NR55" s="2"/>
+      <c r="NS55" s="2"/>
+      <c r="NT55" s="2"/>
+      <c r="NU55" s="2"/>
+      <c r="NV55" s="2"/>
+      <c r="NW55" s="2"/>
+      <c r="NX55" s="2"/>
+      <c r="NY55" s="2"/>
+      <c r="NZ55" s="2"/>
+      <c r="OA55" s="2"/>
+      <c r="OB55" s="2"/>
+      <c r="OC55" s="2"/>
+      <c r="OD55" s="2"/>
+      <c r="OE55" s="2"/>
+      <c r="OF55" s="2"/>
+      <c r="OG55" s="2"/>
+      <c r="OH55" s="2"/>
+      <c r="OI55" s="2"/>
+      <c r="OJ55" s="2"/>
+      <c r="OK55" s="2"/>
+      <c r="OL55" s="2"/>
+      <c r="OM55" s="2"/>
+      <c r="ON55" s="2"/>
+      <c r="OO55" s="2"/>
+      <c r="OP55" s="2"/>
+      <c r="OQ55" s="2"/>
+      <c r="OR55" s="2"/>
+      <c r="OS55" s="2"/>
+      <c r="OT55" s="2"/>
+      <c r="OU55" s="2"/>
+      <c r="OV55" s="2"/>
+      <c r="OW55" s="2"/>
+      <c r="OX55" s="2"/>
+      <c r="OY55" s="2"/>
+      <c r="OZ55" s="2"/>
+      <c r="PA55" s="2"/>
+      <c r="PB55" s="2"/>
+      <c r="PC55" s="2"/>
+      <c r="PD55" s="2"/>
+      <c r="PE55" s="2"/>
+      <c r="PF55" s="2"/>
+      <c r="PG55" s="2"/>
+      <c r="PH55" s="2"/>
+      <c r="PI55" s="2"/>
+      <c r="PJ55" s="2"/>
+      <c r="PK55" s="2"/>
+      <c r="PL55" s="2"/>
+      <c r="PM55" s="2"/>
+      <c r="PN55" s="2"/>
+      <c r="PO55" s="2"/>
+      <c r="PP55" s="2"/>
+      <c r="PQ55" s="2"/>
+      <c r="PR55" s="2"/>
+      <c r="PS55" s="2"/>
+      <c r="PT55" s="2"/>
+      <c r="PU55" s="2"/>
+      <c r="PV55" s="2"/>
+      <c r="PW55" s="2"/>
+      <c r="PX55" s="2"/>
+      <c r="PY55" s="2"/>
+      <c r="PZ55" s="2"/>
+      <c r="QA55" s="2"/>
+      <c r="QB55" s="2"/>
+      <c r="QC55" s="2"/>
+      <c r="QD55" s="2"/>
+      <c r="QE55" s="2"/>
+      <c r="QF55" s="2"/>
+      <c r="QG55" s="2"/>
+      <c r="QH55" s="2"/>
+      <c r="QI55" s="2"/>
+      <c r="QJ55" s="2"/>
+      <c r="QK55" s="2"/>
+      <c r="QL55" s="2"/>
+      <c r="QM55" s="2"/>
+      <c r="QN55" s="2"/>
+      <c r="QO55" s="2"/>
+      <c r="QP55" s="2"/>
+      <c r="QQ55" s="2"/>
+      <c r="QR55" s="2"/>
+      <c r="QS55" s="2"/>
+      <c r="QT55" s="2"/>
+      <c r="QU55" s="2"/>
+      <c r="QV55" s="2"/>
+      <c r="QW55" s="2"/>
+      <c r="QX55" s="2"/>
+      <c r="QY55" s="2"/>
+      <c r="QZ55" s="2"/>
+      <c r="RA55" s="2"/>
+      <c r="RB55" s="2"/>
+      <c r="RC55" s="2"/>
+      <c r="RD55" s="2"/>
+      <c r="RE55" s="2"/>
+      <c r="RF55" s="2"/>
+      <c r="RG55" s="2"/>
+      <c r="RH55" s="2"/>
+      <c r="RI55" s="2"/>
+      <c r="RJ55" s="2"/>
+      <c r="RK55" s="2"/>
+      <c r="RL55" s="2"/>
+      <c r="RM55" s="2"/>
+      <c r="RN55" s="2"/>
+      <c r="RO55" s="2"/>
+      <c r="RP55" s="2"/>
+      <c r="RQ55" s="2"/>
+      <c r="RR55" s="2"/>
+      <c r="RS55" s="2"/>
+      <c r="RT55" s="2"/>
+      <c r="RU55" s="2"/>
+      <c r="RV55" s="2"/>
+      <c r="RW55" s="2"/>
+      <c r="RX55" s="2"/>
+      <c r="RY55" s="2"/>
+      <c r="RZ55" s="2"/>
+      <c r="SA55" s="2"/>
+      <c r="SB55" s="2"/>
+      <c r="SC55" s="2"/>
+      <c r="SD55" s="2"/>
+      <c r="SE55" s="2"/>
+      <c r="SF55" s="2"/>
+      <c r="SG55" s="2"/>
+      <c r="SH55" s="2"/>
+      <c r="SI55" s="2"/>
+      <c r="SJ55" s="2"/>
+      <c r="SK55" s="2"/>
+      <c r="SL55" s="2"/>
+      <c r="SM55" s="2"/>
+      <c r="SN55" s="2"/>
+      <c r="SO55" s="2"/>
+      <c r="SP55" s="2"/>
+      <c r="SQ55" s="2"/>
+      <c r="SR55" s="2"/>
+      <c r="SS55" s="2"/>
+      <c r="ST55" s="2"/>
+      <c r="SU55" s="2"/>
+      <c r="SV55" s="2"/>
+      <c r="SW55" s="2"/>
+      <c r="SX55" s="2"/>
+      <c r="SY55" s="2"/>
+      <c r="SZ55" s="2"/>
+      <c r="TA55" s="2"/>
+      <c r="TB55" s="2"/>
+      <c r="TC55" s="2"/>
+      <c r="TD55" s="2"/>
+      <c r="TE55" s="2"/>
+      <c r="TF55" s="2"/>
+      <c r="TG55" s="2"/>
+      <c r="TH55" s="2"/>
+      <c r="TI55" s="2"/>
+      <c r="TJ55" s="2"/>
+      <c r="TK55" s="2"/>
+      <c r="TL55" s="2"/>
+      <c r="TM55" s="2"/>
+      <c r="TN55" s="2"/>
+      <c r="TO55" s="2"/>
+      <c r="TP55" s="2"/>
+      <c r="TQ55" s="2"/>
+      <c r="TR55" s="2"/>
+      <c r="TS55" s="2"/>
+      <c r="TT55" s="2"/>
+      <c r="TU55" s="2"/>
+      <c r="TV55" s="2"/>
+      <c r="TW55" s="2"/>
+      <c r="TX55" s="2"/>
+      <c r="TY55" s="2"/>
+      <c r="TZ55" s="2"/>
+      <c r="UA55" s="2"/>
+      <c r="UB55" s="2"/>
+      <c r="UC55" s="2"/>
+      <c r="UD55" s="2"/>
+      <c r="UE55" s="2"/>
+      <c r="UF55" s="2"/>
+      <c r="UG55" s="2"/>
+      <c r="UH55" s="2"/>
+      <c r="UI55" s="2"/>
+      <c r="UJ55" s="2"/>
+      <c r="UK55" s="2"/>
+      <c r="UL55" s="2"/>
+      <c r="UM55" s="2"/>
+      <c r="UN55" s="2"/>
+      <c r="UO55" s="2"/>
+      <c r="UP55" s="2"/>
+      <c r="UQ55" s="2"/>
+      <c r="UR55" s="2"/>
+      <c r="US55" s="2"/>
+      <c r="UT55" s="2"/>
+      <c r="UU55" s="2"/>
+      <c r="UV55" s="2"/>
+      <c r="UW55" s="2"/>
+      <c r="UX55" s="2"/>
+      <c r="UY55" s="2"/>
+      <c r="UZ55" s="2"/>
+      <c r="VA55" s="2"/>
+      <c r="VB55" s="2"/>
+      <c r="VC55" s="2"/>
+      <c r="VD55" s="2"/>
+      <c r="VE55" s="2"/>
+      <c r="VF55" s="2"/>
+      <c r="VG55" s="2"/>
+      <c r="VH55" s="2"/>
+      <c r="VI55" s="2"/>
+      <c r="VJ55" s="2"/>
+      <c r="VK55" s="2"/>
+      <c r="VL55" s="2"/>
+      <c r="VM55" s="2"/>
+      <c r="VN55" s="2"/>
+      <c r="VO55" s="2"/>
+      <c r="VP55" s="2"/>
+      <c r="VQ55" s="2"/>
+      <c r="VR55" s="2"/>
+      <c r="VS55" s="2"/>
+      <c r="VT55" s="2"/>
+      <c r="VU55" s="2"/>
+      <c r="VV55" s="2"/>
+      <c r="VW55" s="2"/>
+      <c r="VX55" s="2"/>
+      <c r="VY55" s="2"/>
+      <c r="VZ55" s="2"/>
+      <c r="WA55" s="2"/>
+      <c r="WB55" s="2"/>
+      <c r="WC55" s="2"/>
+      <c r="WD55" s="2"/>
+      <c r="WE55" s="2"/>
+      <c r="WF55" s="2"/>
+      <c r="WG55" s="2"/>
+      <c r="WH55" s="2"/>
+      <c r="WI55" s="2"/>
+      <c r="WJ55" s="2"/>
+      <c r="WK55" s="2"/>
+      <c r="WL55" s="2"/>
+      <c r="WM55" s="2"/>
+      <c r="WN55" s="2"/>
+      <c r="WO55" s="2"/>
+      <c r="WP55" s="2"/>
+      <c r="WQ55" s="2"/>
+      <c r="WR55" s="2"/>
+      <c r="WS55" s="2"/>
+      <c r="WT55" s="2"/>
+      <c r="WU55" s="2"/>
+      <c r="WV55" s="2"/>
+      <c r="WW55" s="2"/>
+      <c r="WX55" s="2"/>
+      <c r="WY55" s="2"/>
+      <c r="WZ55" s="2"/>
+      <c r="XA55" s="2"/>
+      <c r="XB55" s="2"/>
+      <c r="XC55" s="2"/>
+      <c r="XD55" s="2"/>
+      <c r="XE55" s="2"/>
+      <c r="XF55" s="2"/>
+      <c r="XG55" s="2"/>
+      <c r="XH55" s="2"/>
+      <c r="XI55" s="2"/>
+      <c r="XJ55" s="2"/>
+      <c r="XK55" s="2"/>
+      <c r="XL55" s="2"/>
+      <c r="XM55" s="2"/>
+      <c r="XN55" s="2"/>
+      <c r="XO55" s="2"/>
+      <c r="XP55" s="2"/>
+      <c r="XQ55" s="2"/>
+      <c r="XR55" s="2"/>
+      <c r="XS55" s="2"/>
+      <c r="XT55" s="2"/>
+      <c r="XU55" s="2"/>
+      <c r="XV55" s="2"/>
+      <c r="XW55" s="2"/>
+      <c r="XX55" s="2"/>
+      <c r="XY55" s="2"/>
+      <c r="XZ55" s="2"/>
+      <c r="YA55" s="2"/>
+      <c r="YB55" s="2"/>
+      <c r="YC55" s="2"/>
+      <c r="YD55" s="2"/>
+      <c r="YE55" s="2"/>
+      <c r="YF55" s="2"/>
+      <c r="YG55" s="2"/>
+      <c r="YH55" s="2"/>
+      <c r="YI55" s="2"/>
+      <c r="YJ55" s="2"/>
+      <c r="YK55" s="2"/>
+      <c r="YL55" s="2"/>
+      <c r="YM55" s="2"/>
+      <c r="YN55" s="2"/>
+      <c r="YO55" s="2"/>
+      <c r="YP55" s="2"/>
+      <c r="YQ55" s="2"/>
+      <c r="YR55" s="2"/>
+      <c r="YS55" s="2"/>
+      <c r="YT55" s="2"/>
+      <c r="YU55" s="2"/>
+      <c r="YV55" s="2"/>
+      <c r="YW55" s="2"/>
+      <c r="YX55" s="2"/>
+      <c r="YY55" s="2"/>
+      <c r="YZ55" s="2"/>
+      <c r="ZA55" s="2"/>
+      <c r="ZB55" s="2"/>
+      <c r="ZC55" s="2"/>
+      <c r="ZD55" s="2"/>
+      <c r="ZE55" s="2"/>
+      <c r="ZF55" s="2"/>
+      <c r="ZG55" s="2"/>
+      <c r="ZH55" s="2"/>
+      <c r="ZI55" s="2"/>
+      <c r="ZJ55" s="2"/>
+      <c r="ZK55" s="2"/>
+      <c r="ZL55" s="2"/>
+      <c r="ZM55" s="2"/>
+      <c r="ZN55" s="2"/>
+      <c r="ZO55" s="2"/>
+      <c r="ZP55" s="2"/>
+      <c r="ZQ55" s="2"/>
+      <c r="ZR55" s="2"/>
+      <c r="ZS55" s="2"/>
+      <c r="ZT55" s="2"/>
+      <c r="ZU55" s="2"/>
+      <c r="ZV55" s="2"/>
+      <c r="ZW55" s="2"/>
+      <c r="ZX55" s="2"/>
+      <c r="ZY55" s="2"/>
+      <c r="ZZ55" s="2"/>
+      <c r="AAA55" s="2"/>
+      <c r="AAB55" s="2"/>
+      <c r="AAC55" s="2"/>
+      <c r="AAD55" s="2"/>
+      <c r="AAE55" s="2"/>
+      <c r="AAF55" s="2"/>
+      <c r="AAG55" s="2"/>
+      <c r="AAH55" s="2"/>
+      <c r="AAI55" s="2"/>
+      <c r="AAJ55" s="2"/>
+      <c r="AAK55" s="2"/>
+      <c r="AAL55" s="2"/>
+      <c r="AAM55" s="2"/>
+      <c r="AAN55" s="2"/>
+      <c r="AAO55" s="2"/>
+      <c r="AAP55" s="2"/>
+      <c r="AAQ55" s="2"/>
+      <c r="AAR55" s="2"/>
+      <c r="AAS55" s="2"/>
+      <c r="AAT55" s="2"/>
+      <c r="AAU55" s="2"/>
+      <c r="AAV55" s="2"/>
+      <c r="AAW55" s="2"/>
+      <c r="AAX55" s="2"/>
+      <c r="AAY55" s="2"/>
+      <c r="AAZ55" s="2"/>
+      <c r="ABA55" s="2"/>
+      <c r="ABB55" s="2"/>
+      <c r="ABC55" s="2"/>
+      <c r="ABD55" s="2"/>
+      <c r="ABE55" s="2"/>
+      <c r="ABF55" s="2"/>
+      <c r="ABG55" s="2"/>
+      <c r="ABH55" s="2"/>
+      <c r="ABI55" s="2"/>
+      <c r="ABJ55" s="2"/>
+      <c r="ABK55" s="2"/>
+      <c r="ABL55" s="2"/>
+      <c r="ABM55" s="2"/>
+      <c r="ABN55" s="2"/>
+      <c r="ABO55" s="2"/>
+      <c r="ABP55" s="2"/>
+      <c r="ABQ55" s="2"/>
+      <c r="ABR55" s="2"/>
+      <c r="ABS55" s="2"/>
+      <c r="ABT55" s="2"/>
+      <c r="ABU55" s="2"/>
+      <c r="ABV55" s="2"/>
+      <c r="ABW55" s="2"/>
+      <c r="ABX55" s="2"/>
+      <c r="ABY55" s="2"/>
+      <c r="ABZ55" s="2"/>
+      <c r="ACA55" s="2"/>
+      <c r="ACB55" s="2"/>
+      <c r="ACC55" s="2"/>
+      <c r="ACD55" s="2"/>
+      <c r="ACE55" s="2"/>
+      <c r="ACF55" s="2"/>
+      <c r="ACG55" s="2"/>
+      <c r="ACH55" s="2"/>
+      <c r="ACI55" s="2"/>
+      <c r="ACJ55" s="2"/>
+      <c r="ACK55" s="2"/>
+      <c r="ACL55" s="2"/>
+      <c r="ACM55" s="2"/>
+      <c r="ACN55" s="2"/>
+      <c r="ACO55" s="2"/>
+      <c r="ACP55" s="2"/>
+      <c r="ACQ55" s="2"/>
+      <c r="ACR55" s="2"/>
+      <c r="ACS55" s="2"/>
+      <c r="ACT55" s="2"/>
+      <c r="ACU55" s="2"/>
+      <c r="ACV55" s="2"/>
+      <c r="ACW55" s="2"/>
+      <c r="ACX55" s="2"/>
+      <c r="ACY55" s="2"/>
+      <c r="ACZ55" s="2"/>
+      <c r="ADA55" s="2"/>
+      <c r="ADB55" s="2"/>
+      <c r="ADC55" s="2"/>
+      <c r="ADD55" s="2"/>
+      <c r="ADE55" s="2"/>
+      <c r="ADF55" s="2"/>
+      <c r="ADG55" s="2"/>
+      <c r="ADH55" s="2"/>
+      <c r="ADI55" s="2"/>
+      <c r="ADJ55" s="2"/>
+      <c r="ADK55" s="2"/>
+      <c r="ADL55" s="2"/>
+      <c r="ADM55" s="2"/>
+      <c r="ADN55" s="2"/>
+      <c r="ADO55" s="2"/>
+      <c r="ADP55" s="2"/>
+      <c r="ADQ55" s="2"/>
+      <c r="ADR55" s="2"/>
+      <c r="ADS55" s="2"/>
+      <c r="ADT55" s="2"/>
+      <c r="ADU55" s="2"/>
+      <c r="ADV55" s="2"/>
+      <c r="ADW55" s="2"/>
+      <c r="ADX55" s="2"/>
+      <c r="ADY55" s="2"/>
+      <c r="ADZ55" s="2"/>
+      <c r="AEA55" s="2"/>
+      <c r="AEB55" s="2"/>
+      <c r="AEC55" s="2"/>
+      <c r="AED55" s="2"/>
+      <c r="AEE55" s="2"/>
+      <c r="AEF55" s="2"/>
+      <c r="AEG55" s="2"/>
+      <c r="AEH55" s="2"/>
+      <c r="AEI55" s="2"/>
+      <c r="AEJ55" s="2"/>
+      <c r="AEK55" s="2"/>
+      <c r="AEL55" s="2"/>
+      <c r="AEM55" s="2"/>
+      <c r="AEN55" s="2"/>
+      <c r="AEO55" s="2"/>
+      <c r="AEP55" s="2"/>
+      <c r="AEQ55" s="2"/>
+      <c r="AER55" s="2"/>
+      <c r="AES55" s="2"/>
+      <c r="AET55" s="2"/>
+      <c r="AEU55" s="2"/>
+      <c r="AEV55" s="2"/>
+      <c r="AEW55" s="2"/>
+      <c r="AEX55" s="2"/>
+      <c r="AEY55" s="2"/>
+      <c r="AEZ55" s="2"/>
+      <c r="AFA55" s="2"/>
+      <c r="AFB55" s="2"/>
+      <c r="AFC55" s="2"/>
+      <c r="AFD55" s="2"/>
+      <c r="AFE55" s="2"/>
+      <c r="AFF55" s="2"/>
+      <c r="AFG55" s="2"/>
+      <c r="AFH55" s="2"/>
+      <c r="AFI55" s="2"/>
+      <c r="AFJ55" s="2"/>
+      <c r="AFK55" s="2"/>
+      <c r="AFL55" s="2"/>
+      <c r="AFM55" s="2"/>
+      <c r="AFN55" s="2"/>
+      <c r="AFO55" s="2"/>
+      <c r="AFP55" s="2"/>
+      <c r="AFQ55" s="2"/>
+      <c r="AFR55" s="2"/>
+      <c r="AFS55" s="2"/>
+      <c r="AFT55" s="2"/>
+      <c r="AFU55" s="2"/>
+      <c r="AFV55" s="2"/>
+      <c r="AFW55" s="2"/>
+      <c r="AFX55" s="2"/>
+      <c r="AFY55" s="2"/>
+      <c r="AFZ55" s="2"/>
+      <c r="AGA55" s="2"/>
+      <c r="AGB55" s="2"/>
+      <c r="AGC55" s="2"/>
+      <c r="AGD55" s="2"/>
+      <c r="AGE55" s="2"/>
+      <c r="AGF55" s="2"/>
+      <c r="AGG55" s="2"/>
+      <c r="AGH55" s="2"/>
+      <c r="AGI55" s="2"/>
+      <c r="AGJ55" s="2"/>
+      <c r="AGK55" s="2"/>
+      <c r="AGL55" s="2"/>
+      <c r="AGM55" s="2"/>
+      <c r="AGN55" s="2"/>
+      <c r="AGO55" s="2"/>
+      <c r="AGP55" s="2"/>
+      <c r="AGQ55" s="2"/>
+      <c r="AGR55" s="2"/>
+      <c r="AGS55" s="2"/>
+      <c r="AGT55" s="2"/>
+      <c r="AGU55" s="2"/>
+      <c r="AGV55" s="2"/>
+      <c r="AGW55" s="2"/>
+      <c r="AGX55" s="2"/>
+      <c r="AGY55" s="2"/>
+      <c r="AGZ55" s="2"/>
+      <c r="AHA55" s="2"/>
+      <c r="AHB55" s="2"/>
+      <c r="AHC55" s="2"/>
+      <c r="AHD55" s="2"/>
+      <c r="AHE55" s="2"/>
+      <c r="AHF55" s="2"/>
+      <c r="AHG55" s="2"/>
+      <c r="AHH55" s="2"/>
+      <c r="AHI55" s="2"/>
+      <c r="AHJ55" s="2"/>
+      <c r="AHK55" s="2"/>
+      <c r="AHL55" s="2"/>
+      <c r="AHM55" s="2"/>
+      <c r="AHN55" s="2"/>
+      <c r="AHO55" s="2"/>
+      <c r="AHP55" s="2"/>
+      <c r="AHQ55" s="2"/>
+      <c r="AHR55" s="2"/>
+      <c r="AHS55" s="2"/>
+      <c r="AHT55" s="2"/>
+      <c r="AHU55" s="2"/>
+      <c r="AHV55" s="2"/>
+      <c r="AHW55" s="2"/>
+      <c r="AHX55" s="2"/>
+      <c r="AHY55" s="2"/>
+      <c r="AHZ55" s="2"/>
+      <c r="AIA55" s="2"/>
+      <c r="AIB55" s="2"/>
+      <c r="AIC55" s="2"/>
+      <c r="AID55" s="2"/>
+      <c r="AIE55" s="2"/>
+      <c r="AIF55" s="2"/>
+      <c r="AIG55" s="2"/>
+      <c r="AIH55" s="2"/>
+      <c r="AII55" s="2"/>
+      <c r="AIJ55" s="2"/>
+      <c r="AIK55" s="2"/>
+      <c r="AIL55" s="2"/>
+      <c r="AIM55" s="2"/>
+      <c r="AIN55" s="2"/>
+      <c r="AIO55" s="2"/>
+      <c r="AIP55" s="2"/>
+      <c r="AIQ55" s="2"/>
+      <c r="AIR55" s="2"/>
+      <c r="AIS55" s="2"/>
+      <c r="AIT55" s="2"/>
+      <c r="AIU55" s="2"/>
+      <c r="AIV55" s="2"/>
+      <c r="AIW55" s="2"/>
+      <c r="AIX55" s="2"/>
+      <c r="AIY55" s="2"/>
+      <c r="AIZ55" s="2"/>
+      <c r="AJA55" s="2"/>
+      <c r="AJB55" s="2"/>
+      <c r="AJC55" s="2"/>
+      <c r="AJD55" s="2"/>
+      <c r="AJE55" s="2"/>
+      <c r="AJF55" s="2"/>
+      <c r="AJG55" s="2"/>
+      <c r="AJH55" s="2"/>
+      <c r="AJI55" s="2"/>
+      <c r="AJJ55" s="2"/>
+      <c r="AJK55" s="2"/>
+      <c r="AJL55" s="2"/>
+      <c r="AJM55" s="2"/>
+      <c r="AJN55" s="2"/>
+      <c r="AJO55" s="2"/>
+      <c r="AJP55" s="2"/>
+      <c r="AJQ55" s="2"/>
+      <c r="AJR55" s="2"/>
+      <c r="AJS55" s="2"/>
+      <c r="AJT55" s="2"/>
+      <c r="AJU55" s="2"/>
+      <c r="AJV55" s="2"/>
+      <c r="AJW55" s="2"/>
+      <c r="AJX55" s="2"/>
+      <c r="AJY55" s="2"/>
+      <c r="AJZ55" s="2"/>
+      <c r="AKA55" s="2"/>
+      <c r="AKB55" s="2"/>
+      <c r="AKC55" s="2"/>
+      <c r="AKD55" s="2"/>
+      <c r="AKE55" s="2"/>
+      <c r="AKF55" s="2"/>
+      <c r="AKG55" s="2"/>
+      <c r="AKH55" s="2"/>
+      <c r="AKI55" s="2"/>
+      <c r="AKJ55" s="2"/>
+      <c r="AKK55" s="2"/>
+      <c r="AKL55" s="2"/>
+      <c r="AKM55" s="2"/>
+      <c r="AKN55" s="2"/>
+      <c r="AKO55" s="2"/>
+      <c r="AKP55" s="2"/>
+      <c r="AKQ55" s="2"/>
+      <c r="AKR55" s="2"/>
+      <c r="AKS55" s="2"/>
+      <c r="AKT55" s="2"/>
+      <c r="AKU55" s="2"/>
+      <c r="AKV55" s="2"/>
+      <c r="AKW55" s="2"/>
+      <c r="AKX55" s="2"/>
+      <c r="AKY55" s="2"/>
+      <c r="AKZ55" s="2"/>
+      <c r="ALA55" s="2"/>
+      <c r="ALB55" s="2"/>
+      <c r="ALC55" s="2"/>
+      <c r="ALD55" s="2"/>
+      <c r="ALE55" s="2"/>
+      <c r="ALF55" s="2"/>
+      <c r="ALG55" s="2"/>
+      <c r="ALH55" s="2"/>
+      <c r="ALI55" s="2"/>
+      <c r="ALJ55" s="2"/>
+      <c r="ALK55" s="2"/>
+      <c r="ALL55" s="2"/>
+      <c r="ALM55" s="2"/>
+      <c r="ALN55" s="2"/>
+      <c r="ALO55" s="2"/>
+      <c r="ALP55" s="2"/>
+      <c r="ALQ55" s="2"/>
+      <c r="ALR55" s="2"/>
+      <c r="ALS55" s="2"/>
+      <c r="ALT55" s="2"/>
+      <c r="ALU55" s="2"/>
+      <c r="ALV55" s="2"/>
+      <c r="ALW55" s="2"/>
+      <c r="ALX55" s="2"/>
+      <c r="ALY55" s="2"/>
+      <c r="ALZ55" s="2"/>
+      <c r="AMA55" s="2"/>
+      <c r="AMB55" s="2"/>
+      <c r="AMC55" s="2"/>
+      <c r="AMD55" s="2"/>
+      <c r="AME55" s="2"/>
+      <c r="AMF55" s="2"/>
+      <c r="AMG55" s="2"/>
+      <c r="AMH55" s="2"/>
+      <c r="AMI55" s="2"/>
+      <c r="AMJ55" s="2"/>
+      <c r="AMK55" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2320,7 +4386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2466,7 +4532,7 @@
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2482,7 +4548,7 @@
         <v>68</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>84</v>
@@ -2494,7 +4560,7 @@
         <v>88</v>
       </c>
       <c r="K18" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L18" s="27" t="s">
         <v>86</v>
@@ -2773,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -2787,7 +4853,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>124</v>
@@ -3013,12 +5079,12 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>80</v>

</xml_diff>